<commit_message>
chinh sua mot so gd
</commit_message>
<xml_diff>
--- a/LuuFile_Excel/DanhSachSanPham.xlsx
+++ b/LuuFile_Excel/DanhSachSanPham.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="110">
   <si>
     <t/>
   </si>
@@ -53,7 +53,7 @@
     <t>20-09-2023</t>
   </si>
   <si>
-    <t>Singapo</t>
+    <t>Bia</t>
   </si>
   <si>
     <t>Lon</t>
@@ -83,7 +83,7 @@
     <t>22-09-2023</t>
   </si>
   <si>
-    <t>USA</t>
+    <t>Nước ngọt</t>
   </si>
   <si>
     <t>D:\BaiTapLonPTUD_NHOM4\image\NuocNgotPepsi003.jpg</t>
@@ -110,9 +110,6 @@
     <t>28-09-2023</t>
   </si>
   <si>
-    <t>TPHCM, Việt Nam</t>
-  </si>
-  <si>
     <t>D:\BaiTapLonPTUD_NHOM4\image\Bia333005.jpg</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>29-09-2023</t>
   </si>
   <si>
-    <t>Việt Nam</t>
-  </si>
-  <si>
     <t>Chai</t>
   </si>
   <si>
@@ -155,10 +149,10 @@
     <t>11-10-2023</t>
   </si>
   <si>
-    <t>Cửa hàng 4T</t>
-  </si>
-  <si>
-    <t>ph?n</t>
+    <t>Thức ăn</t>
+  </si>
+  <si>
+    <t>Phần</t>
   </si>
   <si>
     <t>D:\BaiTapLonPTUD_NHOM4\image\KhoMucXe008.jpg</t>
@@ -170,9 +164,6 @@
     <t>Xúc xích nướng tiêu</t>
   </si>
   <si>
-    <t>Ph?n</t>
-  </si>
-  <si>
     <t>D:\BaiTapLonPTUD_NHOM4\image\XucXichNuongTieu009.jpg</t>
   </si>
   <si>
@@ -306,6 +297,9 @@
   </si>
   <si>
     <t>Chanh muối</t>
+  </si>
+  <si>
+    <t>Đồ uống</t>
   </si>
   <si>
     <t>Ly</t>
@@ -557,7 +551,7 @@
         <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F8" t="n">
         <v>12000.0</v>
@@ -569,7 +563,7 @@
         <v>9000.0</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
@@ -577,13 +571,13 @@
         <v>6.0</v>
       </c>
       <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
@@ -598,7 +592,7 @@
         <v>15000.0</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10">
@@ -606,28 +600,28 @@
         <v>7.0</v>
       </c>
       <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="F10" t="n">
         <v>12000.0</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H10" t="n">
         <v>6000.0</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11">
@@ -635,28 +629,28 @@
         <v>8.0</v>
       </c>
       <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F11" t="n">
         <v>90000.0</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H11" t="n">
         <v>5000.0</v>
       </c>
       <c r="I11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12">
@@ -664,28 +658,28 @@
         <v>9.0</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F12" t="n">
         <v>40000.0</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H12" t="n">
         <v>2000.0</v>
       </c>
       <c r="I12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
@@ -693,28 +687,28 @@
         <v>10.0</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" t="n">
         <v>35000.0</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H13" t="n">
         <v>600.0</v>
       </c>
       <c r="I13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14">
@@ -722,28 +716,28 @@
         <v>11.0</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F14" t="n">
         <v>90000.0</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H14" t="n">
         <v>700.0</v>
       </c>
       <c r="I14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15">
@@ -751,28 +745,28 @@
         <v>12.0</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F15" t="n">
         <v>170000.0</v>
       </c>
       <c r="G15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H15" t="n">
         <v>200.0</v>
       </c>
       <c r="I15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16">
@@ -780,28 +774,28 @@
         <v>13.0</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F16" t="n">
         <v>210000.0</v>
       </c>
       <c r="G16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H16" t="n">
         <v>800.0</v>
       </c>
       <c r="I16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17">
@@ -809,28 +803,28 @@
         <v>14.0</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F17" t="n">
         <v>80000.0</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H17" t="n">
         <v>400.0</v>
       </c>
       <c r="I17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18">
@@ -838,28 +832,28 @@
         <v>15.0</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F18" t="n">
         <v>150000.0</v>
       </c>
       <c r="G18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H18" t="n">
         <v>250.0</v>
       </c>
       <c r="I18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19">
@@ -867,28 +861,28 @@
         <v>16.0</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F19" t="n">
         <v>120000.0</v>
       </c>
       <c r="G19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H19" t="n">
         <v>1000.0</v>
       </c>
       <c r="I19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20">
@@ -896,28 +890,28 @@
         <v>17.0</v>
       </c>
       <c r="B20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F20" t="n">
         <v>200000.0</v>
       </c>
       <c r="G20" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H20" t="n">
         <v>180.0</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21">
@@ -925,28 +919,28 @@
         <v>18.0</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F21" t="n">
         <v>190000.0</v>
       </c>
       <c r="G21" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H21" t="n">
         <v>200.0</v>
       </c>
       <c r="I21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22">
@@ -954,28 +948,28 @@
         <v>19.0</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F22" t="n">
         <v>240000.0</v>
       </c>
       <c r="G22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H22" t="n">
         <v>100.0</v>
       </c>
       <c r="I22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23">
@@ -983,28 +977,28 @@
         <v>20.0</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F23" t="n">
         <v>130000.0</v>
       </c>
       <c r="G23" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H23" t="n">
         <v>150.0</v>
       </c>
       <c r="I23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24">
@@ -1012,28 +1006,28 @@
         <v>21.0</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F24" t="n">
         <v>10000.0</v>
       </c>
       <c r="G24" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H24" t="n">
         <v>2000.0</v>
       </c>
       <c r="I24" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25">
@@ -1041,28 +1035,28 @@
         <v>22.0</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="F25" t="n">
         <v>60000.0</v>
       </c>
       <c r="G25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H25" t="n">
         <v>100.0</v>
       </c>
       <c r="I25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26">
@@ -1070,28 +1064,28 @@
         <v>23.0</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="F26" t="n">
         <v>40000.0</v>
       </c>
       <c r="G26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H26" t="n">
         <v>100.0</v>
       </c>
       <c r="I26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27">
@@ -1099,28 +1093,28 @@
         <v>24.0</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="F27" t="n">
         <v>30000.0</v>
       </c>
       <c r="G27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H27" t="n">
         <v>150.0</v>
       </c>
       <c r="I27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28">
@@ -1128,28 +1122,28 @@
         <v>25.0</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="F28" t="n">
         <v>45000.0</v>
       </c>
       <c r="G28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H28" t="n">
         <v>200.0</v>
       </c>
       <c r="I28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29">
@@ -1157,28 +1151,28 @@
         <v>26.0</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="F29" t="n">
         <v>90000.0</v>
       </c>
       <c r="G29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H29" t="n">
         <v>80.0</v>
       </c>
       <c r="I29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>